<commit_message>
Start of animation branch/ clean-up
</commit_message>
<xml_diff>
--- a/Session 7 - Python/WagerWarCardGame/Documentation/To Do List.xlsx
+++ b/Session 7 - Python/WagerWarCardGame/Documentation/To Do List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FUBAR1342\Desktop\WagerWarCardGame\WagerWarCardGame\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilbe\Documents\GitHub\PracticalProgramming\Session 7 - Python\WagerWarCardGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CB918E-F6CA-4574-B09B-06F8BD851D15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41700" yWindow="3735" windowWidth="21600" windowHeight="11835" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="38280" yWindow="2280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="11" r:id="rId1"/>
@@ -24,7 +25,6 @@
     <sheet name="WWVictoryWindow" sheetId="9" r:id="rId10"/>
     <sheet name="WWWarConstants" sheetId="10" r:id="rId11"/>
     <sheet name="Deck Rules" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -204,9 +204,6 @@
     <t>Dictionary for card style (k,v) key is name (red, blue) value is file (red.jpg, blue.jpg)</t>
   </si>
   <si>
-    <t>Create progam, to convert resource file to py</t>
-  </si>
-  <si>
     <t>hold gamewindow until on click in overload?</t>
   </si>
   <si>
@@ -268,12 +265,15 @@
   </si>
   <si>
     <t>FIGURE THIS OUT LATER</t>
+  </si>
+  <si>
+    <t>Create progam, to convert resource file to py (Already exists within pyton)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,8 +355,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,6 +370,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,6 +465,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -500,6 +517,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -675,29 +709,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -708,84 +742,90 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A14" sqref="A14:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
@@ -793,7 +833,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>48</v>
       </c>
@@ -801,7 +841,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
@@ -809,23 +849,23 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -837,14 +877,16 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -861,92 +903,92 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A3:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="11">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>2</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B9" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -954,20 +996,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -977,40 +1007,40 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="29.3984375" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="5"/>
+    <col min="1" max="1" width="27.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1021,30 +1051,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="C1:F2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C1" s="12" t="s">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C2" s="12" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1056,40 +1089,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -1107,19 +1140,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="A1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1128,7 +1166,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1138,130 +1176,130 @@
       <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="12" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -1280,15 +1318,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1299,160 +1337,163 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A22" sqref="A22:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="13" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="13" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="12" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="15" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="15" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A17" s="13" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>52</v>
       </c>
@@ -1460,7 +1501,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>50</v>
       </c>
@@ -1468,24 +1509,24 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>53</v>
       </c>
@@ -1493,7 +1534,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>54</v>
       </c>
@@ -1503,12 +1544,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -1521,6 +1556,12 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>